<commit_message>
New class and methods is added 2
</commit_message>
<xml_diff>
--- a/src/main/resources/Admin_Excel.xlsx
+++ b/src/main/resources/Admin_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hp\untitled\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044C2A54-6B08-4D46-94D1-17BBCA0D7401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75820E7-6A92-42B0-BEF0-1A56850D702A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1044" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17832" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PostLogin" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E10"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E483D9-A7A0-4087-9084-3458F12445BA}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>